<commit_message>
ajout tableaux rdt et profils
</commit_message>
<xml_diff>
--- a/RT3/mesures/export_excel/1_continu_SS.xlsx
+++ b/RT3/mesures/export_excel/1_continu_SS.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/LEXAR/Fiches_DQ/RT/RT3/mesures/export_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F3DB9E-68BE-2747-BE57-6A4F4D18DAB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E27450-CD3B-8842-B242-ADB4A5DB5CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuille 1 - 1_continu_SS" sheetId="1" r:id="rId1"/>
+    <sheet name="Continu Lent" sheetId="1" r:id="rId1"/>
     <sheet name="Continu Rapide" sheetId="2" r:id="rId2"/>
     <sheet name="SS1" sheetId="3" r:id="rId3"/>
     <sheet name="SS2" sheetId="4" r:id="rId4"/>
@@ -1290,8 +1290,8 @@
   </sheetPr>
   <dimension ref="A1:B203"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5255,7 +5255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E25A7CEA-F635-4E4F-BB5E-F1E0D966BA3E}">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
rapports fiche 3 presque terminés
</commit_message>
<xml_diff>
--- a/RT3/mesures/export_excel/1_continu_SS.xlsx
+++ b/RT3/mesures/export_excel/1_continu_SS.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/LEXAR/Fiches_DQ/RT/RT3/mesures/export_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E27450-CD3B-8842-B242-ADB4A5DB5CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE41904-FDC1-6242-9FF7-2325EC2B8E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Continu Lent" sheetId="1" r:id="rId1"/>
     <sheet name="Continu Rapide" sheetId="2" r:id="rId2"/>
-    <sheet name="SS1" sheetId="3" r:id="rId3"/>
-    <sheet name="SS2" sheetId="4" r:id="rId4"/>
-    <sheet name="SS3" sheetId="5" r:id="rId5"/>
-    <sheet name="SS4" sheetId="6" r:id="rId6"/>
-    <sheet name="SS5" sheetId="7" r:id="rId7"/>
+    <sheet name="0,1_0,5_1" sheetId="3" r:id="rId3"/>
+    <sheet name="0,1_0,5_0,5" sheetId="4" r:id="rId4"/>
+    <sheet name="0,1_0,5_3" sheetId="5" r:id="rId5"/>
+    <sheet name="0,5_1_1" sheetId="6" r:id="rId6"/>
+    <sheet name="0,05_0,2_1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -3626,7 +3626,7 @@
   <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection sqref="A1:B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5256,7 +5256,7 @@
   <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection sqref="A1:B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6302,7 +6302,7 @@
   <dimension ref="A1:B203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B203"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>